<commit_message>
integrating web crawler and updated with gpt
</commit_message>
<xml_diff>
--- a/Reference_files/queries.xlsx
+++ b/Reference_files/queries.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ANKITA</t>
+          <t>Reliance Retail Limited.</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ANKITA</t>
+          <t>iPhone XR 128GB</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>iPhone</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CNB 30W Fast Charging Type C Rapidly Adapter Compatible with Google Pixel 8 Pro/8, 7 Pro/7/7A, 6 Pro/6/6A/5/4, Tablet/Buds/Chrome Books/Laptop and Other USB C Mobile Device Support 30 W | B0DDYC12SW ( A GOOGLE 01 )</t>
+          <t>iPhone XR 128GB</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-01-05</t>
+          <t>2019-08-03</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>05.01.2025</t>
+          <t>2019-08-03</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>07AZAPA3803E1Z5</t>
+          <t>29AABCR1718E1ZL</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>IN-2529</t>
+          <t>8884136002703082019</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>₹699.00</t>
+          <t>The total amount is Rs 63591.22.</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>No discount provided.</t>
+          <t>Discount: Rs 1297.78</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>₹106.63</t>
+          <t>15.08</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>18%</t>
+          <t>0.00%</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ANKITA* 4649/C -75, Street No. 10, New ModernShahdara, Near Sanjay Provisional Store, Budhbazar, Delhi - 110032NEW DELHI, DELHI, 110032IN</t>
+          <t>#LG10, Phoenix Market City, Opp. Mahadevapura CMC Office, Whitefield Road, Bangalore - 560048.</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1/57/A/194 , sri Aurobindo Residency, 9, sriram nagar road,Sri Ram nagar HYDERABAD, TELANGANA, 500084</t>
+          <t>Customer Address:V SRINIVASUFlat No: 404Flr No: 4TH FLOORWing: B BLOCKBldg: ALEMBIC URBAN FORESTSoc: AB VAJPAYEE ROADSec/Loc: .Plot No: CHENNASANDRA MAIN ROADStreet: OPP TO WHITEFIELD GLOBAL SCHOOLArea: KADUGODICity: BANGALORE EASTState: KARNATAKAPinCode: 560067Contact# 9886642984NEELIMA_VE@YAHOO.CO.INRelationship ID: 9886642984</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>LoukyaFlat 302 , mahadev enclave, Janaki ram street,sapthagiri colonyKARIMNAGAR, TELANGANA, 505001IN</t>
+          <t>Customer Address:V SRINIVASUFlat No: 404Flr No: 4TH FLOORWing: B BLOCKBldg: ALEMBIC URBAN FORESTSoc: AB VAJPAYEE ROADSec/Loc: .Plot No: CHENNASANDRA MAIN ROADStreet: OPP TO WHITEFIELD GLOBAL SCHOOLArea: KADUGODICity: BANGALORE EASTState: KARNATAKAPinCode: 560067</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ANKITA* 4649/C -75, Street No. 10, New ModernShahdara, Near Sanjay Provisional Store, Budhbazar, Delhi - 110032NEW DELHI, DELHI, 110032IN</t>
+          <t>#LG10, Phoenix Market City, Opp. Mahadevapura CMC Office, Whitefield Road, Bangalore - 560048.</t>
         </is>
       </c>
     </row>
@@ -752,7 +752,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Syam</t>
+          <t>V SRINIVASU</t>
         </is>
       </c>
     </row>
@@ -769,7 +769,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>AZAPA3803E</t>
+          <t>U01100MH1999PLC120563</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>UPI</t>
+          <t>EMI</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CNB 30W Fast Charging Type C Rapidly Adapter</t>
+          <t>iPhone XR 128GB</t>
         </is>
       </c>
     </row>
@@ -816,7 +816,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2020-08-02</t>
         </is>
       </c>
     </row>

</xml_diff>